<commit_message>
mejorar apuntes y añadido cnn con mejoras
</commit_message>
<xml_diff>
--- a/Horas_invertidas.xlsx
+++ b/Horas_invertidas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vadim\Desktop\TFG\Machine-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4F0AEC-E0E7-43AB-BFC1-F9D3048DCD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E0255C-0A66-4113-9978-70D08CFE15B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Comentarios</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>● Leer hasta la página 183. ● Estudio de los ejemplos mnist de redes convolucionales con keras y pytorch (apéndice B)</t>
+  </si>
+  <si>
+    <t>● Leer hasta la página 215 ●Estudio de los ejemplos de predicción stock market con RNN keras y pytorch (apéndice C)</t>
+  </si>
+  <si>
+    <t>Sábado</t>
+  </si>
+  <si>
+    <t>●Leer hasta la página 280 del libro ●Avanzar apuntes</t>
   </si>
 </sst>
 </file>
@@ -470,7 +479,7 @@
   <dimension ref="B1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,7 +570,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="10"/>
       <c r="C6" s="7" t="s">
         <v>10</v>
@@ -569,8 +578,12 @@
       <c r="D6" s="8">
         <v>45351</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="9"/>
+      <c r="E6" s="7">
+        <v>3</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="G6" s="11"/>
     </row>
     <row r="7" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -585,82 +598,126 @@
       <c r="F7" s="9"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="9"/>
+      <c r="C8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="8">
+        <v>45353</v>
+      </c>
+      <c r="E8" s="7">
+        <v>3</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="G8" s="11"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="10"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
+      <c r="C9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="8">
+        <v>45354</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
       <c r="G9" s="11"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
+      <c r="C10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="8">
+        <v>45355</v>
+      </c>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
       <c r="G10" s="11"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
+      <c r="C11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="8">
+        <v>45356</v>
+      </c>
       <c r="E11" s="7"/>
       <c r="F11" s="9"/>
       <c r="G11" s="11"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
+      <c r="C12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="8">
+        <v>45357</v>
+      </c>
       <c r="E12" s="7"/>
       <c r="F12" s="9"/>
       <c r="G12" s="11"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
+      <c r="C13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="8">
+        <v>45358</v>
+      </c>
       <c r="E13" s="7"/>
       <c r="F13" s="9"/>
       <c r="G13" s="11"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="8">
+        <v>45359</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="9"/>
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="10"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
+      <c r="C15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="8">
+        <v>45360</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="9"/>
       <c r="G15" s="11"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
+      <c r="C16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="8">
+        <v>45361</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="9"/>
       <c r="G16" s="11"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
+      <c r="C17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="8">
+        <v>45362</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="9"/>
       <c r="G17" s="11"/>

</xml_diff>

<commit_message>
añadido huggingface tl y actualizadas horas
</commit_message>
<xml_diff>
--- a/Horas_invertidas.xlsx
+++ b/Horas_invertidas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vadim\Desktop\TFG\Machine-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B1D73A-8FA1-4DB3-8A6A-B7B54FE26DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED4B54F-8280-40CB-B9B6-E60D5F2FA28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Comentarios</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>●Leer hasta la página 370 ●Estudio de los ejemplos FCN con TL en keras y pytorch (apéndice E)</t>
+  </si>
+  <si>
+    <t>●Leer hasta la página 404 ● Estudio de los ejemplos transformer  con TL en keras y pytorch (apéndice F)</t>
   </si>
 </sst>
 </file>
@@ -499,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +682,7 @@
       </c>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
       <c r="C12" s="7" t="s">
         <v>7</v>
@@ -687,20 +690,24 @@
       <c r="D12" s="8">
         <v>45357</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="9"/>
+      <c r="E12" s="7">
+        <v>4</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="G12" s="11"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="13">
         <v>45358</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="9"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="11"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
apuntes finales libro y añadidos datos del curso de verano
</commit_message>
<xml_diff>
--- a/Horas_invertidas.xlsx
+++ b/Horas_invertidas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vadim\Desktop\TFG\Machine-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED4B54F-8280-40CB-B9B6-E60D5F2FA28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9775D964-D34C-4C17-9DAE-6F24CF8240B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Comentarios</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>●Leer hasta la página 404 ● Estudio de los ejemplos transformer  con TL en keras y pytorch (apéndice F)</t>
+  </si>
+  <si>
+    <t>●Libro terminado ●Estudio ejemplo transformer keras con hugging face</t>
   </si>
 </sst>
 </file>
@@ -503,7 +506,7 @@
   <dimension ref="B1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +713,7 @@
       <c r="F13" s="14"/>
       <c r="G13" s="11"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
       <c r="C14" s="7" t="s">
         <v>11</v>
@@ -718,8 +721,12 @@
       <c r="D14" s="8">
         <v>45359</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="9"/>
+      <c r="E14" s="7">
+        <v>3</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
curso de verano cap2
</commit_message>
<xml_diff>
--- a/Horas_invertidas.xlsx
+++ b/Horas_invertidas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vadim\Desktop\TFG\Machine-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9775D964-D34C-4C17-9DAE-6F24CF8240B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEC2220-B7FE-4E52-8568-F4EADC7F3EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>Comentarios</t>
   </si>
@@ -94,13 +94,19 @@
   </si>
   <si>
     <t>●Libro terminado ●Estudio ejemplo transformer keras con hugging face</t>
+  </si>
+  <si>
+    <t>● Curso de verano del moodle, capítulo 1</t>
+  </si>
+  <si>
+    <t>● Curso de verano del moodle, capítulo 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +131,14 @@
     <font>
       <sz val="11"/>
       <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -183,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -221,6 +235,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -506,7 +523,7 @@
   <dimension ref="B1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,8 +754,12 @@
       <c r="D15" s="8">
         <v>45360</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="9"/>
+      <c r="E15" s="7">
+        <v>2</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="G15" s="11"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
@@ -749,8 +770,12 @@
       <c r="D16" s="8">
         <v>45361</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="9"/>
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="G16" s="11"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -762,45 +787,65 @@
         <v>45362</v>
       </c>
       <c r="E17" s="7"/>
-      <c r="F17" s="9"/>
+      <c r="F17" s="15"/>
       <c r="G17" s="11"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
+      <c r="C18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="8">
+        <v>45363</v>
+      </c>
       <c r="E18" s="7"/>
       <c r="F18" s="9"/>
       <c r="G18" s="11"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
+      <c r="C19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="8">
+        <v>45364</v>
+      </c>
       <c r="E19" s="7"/>
       <c r="F19" s="9"/>
       <c r="G19" s="11"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
+      <c r="C20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="8">
+        <v>45365</v>
+      </c>
       <c r="E20" s="7"/>
       <c r="F20" s="9"/>
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
+      <c r="C21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="8">
+        <v>45366</v>
+      </c>
       <c r="E21" s="7"/>
       <c r="F21" s="9"/>
       <c r="G21" s="11"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
+      <c r="C22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="8">
+        <v>45367</v>
+      </c>
       <c r="E22" s="7"/>
       <c r="F22" s="9"/>
       <c r="G22" s="11"/>

</xml_diff>

<commit_message>
añadido guardado del history y añado time elapsed
</commit_message>
<xml_diff>
--- a/Horas_invertidas.xlsx
+++ b/Horas_invertidas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vadim\Desktop\TFG\Machine-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF41C0F-45CF-4697-9C29-73B7EE3D384D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AA84BF-79D3-451A-879C-9EEACCA762C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="60" windowWidth="26385" windowHeight="13665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="38">
   <si>
     <t>Comentarios</t>
   </si>
@@ -563,7 +563,7 @@
   <dimension ref="B1:G88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,8 +1442,12 @@
       <c r="D59" s="3">
         <v>45404</v>
       </c>
-      <c r="E59" s="13"/>
-      <c r="F59" s="15"/>
+      <c r="E59" s="13">
+        <v>2</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="G59" s="6"/>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
@@ -1454,8 +1458,12 @@
       <c r="D60" s="3">
         <v>45405</v>
       </c>
-      <c r="E60" s="13"/>
-      <c r="F60" s="15"/>
+      <c r="E60" s="13">
+        <v>2</v>
+      </c>
+      <c r="F60" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="G60" s="6"/>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.25">
@@ -1466,8 +1474,12 @@
       <c r="D61" s="3">
         <v>45406</v>
       </c>
-      <c r="E61" s="13"/>
-      <c r="F61" s="15"/>
+      <c r="E61" s="13">
+        <v>1</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="G61" s="6"/>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
@@ -1478,32 +1490,36 @@
       <c r="D62" s="3">
         <v>45407</v>
       </c>
-      <c r="E62" s="13"/>
-      <c r="F62" s="15"/>
+      <c r="E62" s="13">
+        <v>1</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="G62" s="6"/>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D63" s="8">
         <v>45408</v>
       </c>
-      <c r="E63" s="13"/>
-      <c r="F63" s="15"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="16"/>
       <c r="G63" s="6"/>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D64" s="8">
         <v>45409</v>
       </c>
-      <c r="E64" s="13"/>
-      <c r="F64" s="15"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="16"/>
       <c r="G64" s="6"/>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>